<commit_message>
nuevo formato de documento
</commit_message>
<xml_diff>
--- a/public/formatos_academicos/F-DA-GA-01 Presentación de la asignatura.xlsx
+++ b/public/formatos_academicos/F-DA-GA-01 Presentación de la asignatura.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B889029C-F4F8-4ECC-8FE9-7CF19E62407E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1E949A-2BF1-4853-829A-1D538446509F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="933" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,21 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Presentación de la Asignatura</t>
   </si>
@@ -43,40 +34,7 @@
     <t>No.</t>
   </si>
   <si>
-    <t>Actividades a realizar</t>
-  </si>
-  <si>
-    <t>Presentación del Profesor</t>
-  </si>
-  <si>
-    <t>Presentación del Programa de la Asignatura</t>
-  </si>
-  <si>
-    <t>Forma de evaluar</t>
-  </si>
-  <si>
-    <t>Políticas de clase</t>
-  </si>
-  <si>
-    <t>Instrucciones o Anotaciones</t>
-  </si>
-  <si>
-    <t>Horario de clases</t>
-  </si>
-  <si>
-    <t>El horario semanal de la asignatura es:</t>
-  </si>
-  <si>
     <t>Matrícula</t>
-  </si>
-  <si>
-    <t>El profesor debe decir su nombre, su formación profesional, académica y laboral, así como su ubicación en la UTM, horarios de atención y datos de localización.</t>
-  </si>
-  <si>
-    <t>El profesor debe dar a conocer, la competencia, el objetivo, las unidades temáticas y las fuentes bibliográficas.</t>
-  </si>
-  <si>
-    <t>Las políticas de la clase son las siguientes:</t>
   </si>
   <si>
     <t>Programa Educativo</t>
@@ -101,9 +59,6 @@
   </si>
   <si>
     <t>Nombre de la Asignatura</t>
-  </si>
-  <si>
-    <t>Observaciones</t>
   </si>
   <si>
     <t>Registrar la matrícula, nombre completo y firma de cada estudiante del grupo que recibió la información:</t>
@@ -155,14 +110,153 @@
 Subdirección de Carrera</t>
   </si>
   <si>
-    <t>El profesor explicará en qué consiste el portafolio de evidencias y los instrumentos de evaluación de la Asignatura.</t>
+    <t>Instrucción de trabajo</t>
+  </si>
+  <si>
+    <t>Ponderación (%)</t>
+  </si>
+  <si>
+    <t>Instrumentos de evaluación</t>
+  </si>
+  <si>
+    <t>Unidad de aprendizaje</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">El docente deberá informar el primer día de clases a cada uno de sus grupos lo siguiente:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Presentación del docente:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Nombre completo, formación profesional, académica y laboral y el horario de clases.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Presentación de la asignatura: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nombre de la asignatura, la competencia a la que pertenece y su objetivo, unidades de aprendizaje y referencias bibliográficas y digitales (Información extraída del Programa de Asignatura).</t>
+    </r>
+  </si>
+  <si>
+    <t>Nota: El docente deberá asegurar que toda la información plasmada en este formato debe estar escrita en la libreta de cada estudiante.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Atención al estudiante
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Escribir los horarios de atención y/o asesoría, su ubicación en la Universidad (si aplica) y por lo menos un dato de localización digital como el número de teléfono del profesor y/o el correo institucional</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Forma de evaluación por competencias </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Escribir de acuerdo con la Planeación Didáctica del Programa de Asignatura</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Políticas de clase </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Escribir los acuerdos que se establezcan con el grupo para procurar un ambiente adecuado para impartir la clase</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +373,40 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -294,7 +422,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -330,19 +458,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -445,15 +560,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -580,7 +686,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -592,13 +698,28 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -607,10 +728,76 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -622,9 +809,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -643,52 +828,9 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -697,7 +839,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -720,7 +862,7 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
@@ -754,7 +896,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -766,10 +908,6 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -778,10 +916,6 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -797,6 +931,49 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -813,83 +990,174 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -897,46 +1165,16 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -951,10 +1189,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1374,10 +1612,10 @@
   <sheetPr codeName="Hoja1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:P1"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1392,12 +1630,12 @@
     <col min="8" max="8" width="6.7265625" style="1" customWidth="1"/>
     <col min="9" max="9" width="1" style="1" customWidth="1"/>
     <col min="10" max="10" width="4.26953125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="4.81640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.1796875" style="1" customWidth="1"/>
     <col min="12" max="12" width="23.81640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="1" style="1" customWidth="1"/>
     <col min="14" max="14" width="4.54296875" style="1" customWidth="1"/>
     <col min="15" max="15" width="6.54296875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="24.26953125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="21.54296875" style="1" customWidth="1"/>
     <col min="17" max="255" width="11.453125" style="1"/>
     <col min="256" max="256" width="5.1796875" style="1" customWidth="1"/>
     <col min="257" max="257" width="4.54296875" style="1" customWidth="1"/>
@@ -2474,26 +2712,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="31" t="s">
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-    </row>
-    <row r="2" spans="1:16" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+    </row>
+    <row r="2" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -2512,27 +2750,27 @@
       <c r="P2" s="13"/>
     </row>
     <row r="3" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
+      <c r="A3" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="13"/>
-      <c r="L3" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
+      <c r="L3" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
       <c r="O3" s="13"/>
       <c r="P3" s="14" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2555,29 +2793,32 @@
     </row>
     <row r="5" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="19"/>
       <c r="D5" s="17" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="19"/>
       <c r="G5" s="11"/>
       <c r="H5" s="17" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="19"/>
       <c r="K5" s="13"/>
       <c r="L5" s="20" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="M5" s="21"/>
       <c r="N5" s="19"/>
       <c r="O5" s="13"/>
-      <c r="P5" s="22"/>
+      <c r="P5" s="32">
+        <f ca="1">TODAY()</f>
+        <v>45909</v>
+      </c>
     </row>
     <row r="6" spans="1:16" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
@@ -2599,30 +2840,30 @@
     </row>
     <row r="7" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="19"/>
       <c r="D7" s="17" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="19"/>
       <c r="G7" s="11"/>
       <c r="H7" s="17" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="I7" s="20"/>
       <c r="J7" s="19"/>
       <c r="K7" s="13"/>
       <c r="L7" s="20" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="M7" s="21"/>
       <c r="N7" s="19"/>
       <c r="O7" s="13"/>
       <c r="P7" s="14" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="3.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2645,29 +2886,29 @@
     </row>
     <row r="9" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="23"/>
+        <v>16</v>
+      </c>
+      <c r="B9" s="22"/>
       <c r="C9" s="19"/>
-      <c r="D9" s="24" t="s">
-        <v>33</v>
+      <c r="D9" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="19"/>
       <c r="G9" s="13"/>
       <c r="H9" s="17" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="I9" s="13"/>
       <c r="J9" s="19"/>
       <c r="K9" s="13"/>
       <c r="L9" s="20" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="M9" s="21"/>
       <c r="N9" s="19"/>
       <c r="O9" s="13"/>
-      <c r="P9" s="25"/>
+      <c r="P9" s="19"/>
     </row>
     <row r="10" spans="1:16" ht="4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
@@ -2689,9 +2930,9 @@
     </row>
     <row r="11" spans="1:16" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="23"/>
+        <v>17</v>
+      </c>
+      <c r="B11" s="22"/>
       <c r="C11" s="19"/>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -2707,7 +2948,7 @@
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
     </row>
-    <row r="12" spans="1:16" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="6.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
@@ -2726,583 +2967,600 @@
       <c r="P12" s="13"/>
     </row>
     <row r="13" spans="1:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="68" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="68"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="62"/>
-      <c r="P13" s="63"/>
-    </row>
-    <row r="14" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="50"/>
+    </row>
+    <row r="14" spans="1:16" ht="6.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
-      <c r="B14" s="27"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-    </row>
-    <row r="15" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-    </row>
-    <row r="16" spans="1:16" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-    </row>
-    <row r="17" spans="1:16" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="66" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="67"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="67"/>
-      <c r="L17" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="M17" s="64"/>
-      <c r="N17" s="64"/>
-      <c r="O17" s="64"/>
-      <c r="P17" s="65"/>
-    </row>
-    <row r="18" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="M18" s="47"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="48"/>
-    </row>
-    <row r="19" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="48"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+    </row>
+    <row r="15" spans="1:16" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="53"/>
+      <c r="O15" s="53"/>
+      <c r="P15" s="54"/>
+    </row>
+    <row r="16" spans="1:16" ht="62.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="57"/>
+    </row>
+    <row r="17" spans="1:16" ht="7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="58"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="58"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="58"/>
+    </row>
+    <row r="18" spans="1:16" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="61"/>
+    </row>
+    <row r="19" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="65"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="66"/>
+      <c r="O19" s="66"/>
+      <c r="P19" s="67"/>
     </row>
     <row r="20" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="59" t="s">
-        <v>9</v>
-      </c>
-      <c r="M20" s="59"/>
-      <c r="N20" s="59"/>
-      <c r="O20" s="59"/>
-      <c r="P20" s="60"/>
-    </row>
-    <row r="21" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="43"/>
-      <c r="O21" s="43"/>
-      <c r="P21" s="44"/>
-    </row>
-    <row r="22" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="44"/>
-    </row>
-    <row r="23" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="37"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="43"/>
-      <c r="P23" s="44"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="64"/>
+    </row>
+    <row r="21" spans="1:16" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="68"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="69"/>
+      <c r="N21" s="69"/>
+      <c r="O21" s="69"/>
+      <c r="P21" s="70"/>
+    </row>
+    <row r="22" spans="1:16" ht="6.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="58"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="58"/>
+      <c r="K22" s="58"/>
+      <c r="L22" s="58"/>
+      <c r="M22" s="58"/>
+      <c r="N22" s="58"/>
+      <c r="O22" s="58"/>
+      <c r="P22" s="58"/>
+    </row>
+    <row r="23" spans="1:16" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="72"/>
+      <c r="K23" s="72"/>
+      <c r="L23" s="72"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="72"/>
+      <c r="P23" s="73"/>
     </row>
     <row r="24" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="43"/>
-      <c r="P24" s="44"/>
+      <c r="A24" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="40"/>
+      <c r="P24" s="34" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="25" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="M25" s="59"/>
-      <c r="N25" s="59"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="60"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="30"/>
     </row>
     <row r="26" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="37"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="43"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="44"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="30"/>
     </row>
     <row r="27" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="37"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="43"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="44"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="36"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="30"/>
     </row>
     <row r="28" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="39"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="40"/>
-      <c r="K28" s="40"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="43"/>
-      <c r="N28" s="43"/>
-      <c r="O28" s="43"/>
-      <c r="P28" s="44"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="36"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="30"/>
     </row>
     <row r="29" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="39"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="43"/>
-      <c r="O29" s="43"/>
-      <c r="P29" s="44"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="30"/>
     </row>
     <row r="30" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="41"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="45"/>
-      <c r="P30" s="46"/>
-    </row>
-    <row r="31" spans="1:16" ht="9.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-    </row>
-    <row r="32" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
-      <c r="N32" s="33"/>
-      <c r="O32" s="33"/>
-      <c r="P32" s="33"/>
-    </row>
-    <row r="33" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="52"/>
-      <c r="B33" s="52"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="52"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="52"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52"/>
-      <c r="N33" s="52"/>
-      <c r="O33" s="52"/>
-      <c r="P33" s="52"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="35"/>
+      <c r="P30" s="31"/>
+    </row>
+    <row r="31" spans="1:16" ht="5.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:16" ht="35.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="80"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="80"/>
+      <c r="L32" s="80"/>
+      <c r="M32" s="80"/>
+      <c r="N32" s="80"/>
+      <c r="O32" s="80"/>
+      <c r="P32" s="81"/>
+    </row>
+    <row r="33" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="82"/>
+      <c r="B33" s="83"/>
+      <c r="C33" s="83"/>
+      <c r="D33" s="83"/>
+      <c r="E33" s="83"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="83"/>
+      <c r="H33" s="83"/>
+      <c r="I33" s="83"/>
+      <c r="J33" s="83"/>
+      <c r="K33" s="83"/>
+      <c r="L33" s="83"/>
+      <c r="M33" s="83"/>
+      <c r="N33" s="83"/>
+      <c r="O33" s="83"/>
+      <c r="P33" s="84"/>
     </row>
     <row r="34" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="52"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="52"/>
-      <c r="P34" s="52"/>
+      <c r="A34" s="92"/>
+      <c r="B34" s="93"/>
+      <c r="C34" s="93"/>
+      <c r="D34" s="93"/>
+      <c r="E34" s="93"/>
+      <c r="F34" s="93"/>
+      <c r="G34" s="93"/>
+      <c r="H34" s="93"/>
+      <c r="I34" s="93"/>
+      <c r="J34" s="93"/>
+      <c r="K34" s="93"/>
+      <c r="L34" s="93"/>
+      <c r="M34" s="93"/>
+      <c r="N34" s="93"/>
+      <c r="O34" s="93"/>
+      <c r="P34" s="94"/>
     </row>
     <row r="35" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="52"/>
-      <c r="D35" s="52"/>
-      <c r="E35" s="52"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52"/>
-      <c r="I35" s="52"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="52"/>
-      <c r="L35" s="52"/>
-      <c r="M35" s="52"/>
-      <c r="N35" s="52"/>
-      <c r="O35" s="52"/>
-      <c r="P35" s="52"/>
-    </row>
-    <row r="36" spans="1:16" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-    </row>
-    <row r="37" spans="1:16" ht="48.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="35"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="N37" s="54"/>
-      <c r="O37" s="54"/>
-      <c r="P37" s="55"/>
-    </row>
-    <row r="38" spans="1:16" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="49"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50"/>
-      <c r="G38" s="50"/>
-      <c r="H38" s="50"/>
-      <c r="I38" s="50"/>
-      <c r="J38" s="50"/>
-      <c r="K38" s="51"/>
+      <c r="A35" s="82"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="83"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="83"/>
+      <c r="F35" s="83"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="83"/>
+      <c r="I35" s="83"/>
+      <c r="J35" s="83"/>
+      <c r="K35" s="83"/>
+      <c r="L35" s="83"/>
+      <c r="M35" s="83"/>
+      <c r="N35" s="83"/>
+      <c r="O35" s="83"/>
+      <c r="P35" s="84"/>
+    </row>
+    <row r="36" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="77"/>
+      <c r="B36" s="78"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="78"/>
+      <c r="I36" s="78"/>
+      <c r="J36" s="78"/>
+      <c r="K36" s="78"/>
+      <c r="L36" s="78"/>
+      <c r="M36" s="78"/>
+      <c r="N36" s="78"/>
+      <c r="O36" s="78"/>
+      <c r="P36" s="79"/>
+    </row>
+    <row r="37" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="85" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="85"/>
+      <c r="C37" s="85"/>
+      <c r="D37" s="85"/>
+      <c r="E37" s="85"/>
+      <c r="F37" s="85"/>
+      <c r="G37" s="85"/>
+      <c r="H37" s="85"/>
+      <c r="I37" s="85"/>
+      <c r="J37" s="85"/>
+      <c r="K37" s="85"/>
+      <c r="L37" s="85"/>
+      <c r="M37" s="85"/>
+      <c r="N37" s="85"/>
+      <c r="O37" s="85"/>
+      <c r="P37" s="85"/>
+    </row>
+    <row r="38" spans="1:16" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
       <c r="L38" s="13"/>
-      <c r="M38" s="56"/>
-      <c r="N38" s="57"/>
-      <c r="O38" s="57"/>
-      <c r="P38" s="58"/>
-    </row>
-    <row r="39" spans="1:16" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="13"/>
-      <c r="K39" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
+    </row>
+    <row r="39" spans="1:16" ht="52" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="46"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="47"/>
       <c r="L39" s="13"/>
-      <c r="M39" s="13"/>
-      <c r="N39" s="13"/>
-      <c r="O39" s="13"/>
-      <c r="P39" s="13"/>
-    </row>
-    <row r="40" spans="1:16" ht="14" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
+      <c r="M39" s="86" t="s">
+        <v>26</v>
+      </c>
+      <c r="N39" s="87"/>
+      <c r="O39" s="87"/>
+      <c r="P39" s="88"/>
+    </row>
+    <row r="40" spans="1:16" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="74"/>
+      <c r="B40" s="75"/>
+      <c r="C40" s="75"/>
+      <c r="D40" s="75"/>
+      <c r="E40" s="75"/>
+      <c r="F40" s="75"/>
+      <c r="G40" s="75"/>
+      <c r="H40" s="75"/>
+      <c r="I40" s="75"/>
+      <c r="J40" s="75"/>
+      <c r="K40" s="76"/>
       <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="13"/>
-      <c r="P40" s="29" t="s">
-        <v>30</v>
+      <c r="M40" s="89"/>
+      <c r="N40" s="90"/>
+      <c r="O40" s="90"/>
+      <c r="P40" s="91"/>
+    </row>
+    <row r="41" spans="1:16" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+    </row>
+    <row r="42" spans="1:16" ht="14" x14ac:dyDescent="0.3">
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="27" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="L25:P25"/>
-    <mergeCell ref="L27:P27"/>
-    <mergeCell ref="L26:P26"/>
-    <mergeCell ref="H13:P13"/>
-    <mergeCell ref="L17:P17"/>
-    <mergeCell ref="L23:P23"/>
-    <mergeCell ref="A20:K24"/>
-    <mergeCell ref="L20:P20"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="L15:P15"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A38:K38"/>
-    <mergeCell ref="A34:P34"/>
+  <mergeCells count="38">
+    <mergeCell ref="A40:K40"/>
+    <mergeCell ref="A36:P36"/>
     <mergeCell ref="A32:P32"/>
     <mergeCell ref="A33:P33"/>
+    <mergeCell ref="A37:P37"/>
+    <mergeCell ref="M39:P40"/>
+    <mergeCell ref="A34:P34"/>
     <mergeCell ref="A35:P35"/>
-    <mergeCell ref="M37:P38"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="K1:P1"/>
     <mergeCell ref="L3:N3"/>
     <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A37:K37"/>
-    <mergeCell ref="A25:K30"/>
-    <mergeCell ref="L28:P28"/>
-    <mergeCell ref="L30:P30"/>
-    <mergeCell ref="L29:P29"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="L18:P18"/>
-    <mergeCell ref="A19:K19"/>
-    <mergeCell ref="L19:P19"/>
-    <mergeCell ref="L21:P21"/>
-    <mergeCell ref="L22:P22"/>
-    <mergeCell ref="L24:P24"/>
+    <mergeCell ref="A39:K39"/>
+    <mergeCell ref="H13:P13"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A15:P15"/>
+    <mergeCell ref="A16:P16"/>
+    <mergeCell ref="A17:P17"/>
+    <mergeCell ref="A18:P18"/>
+    <mergeCell ref="A20:P20"/>
+    <mergeCell ref="A22:P22"/>
+    <mergeCell ref="A19:P19"/>
+    <mergeCell ref="A21:P21"/>
+    <mergeCell ref="A23:P23"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="I24:O24"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="I28:O28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="I29:O29"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="I30:O30"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="I25:O25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="I26:O26"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="I27:O27"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.26" footer="0.25"/>
-  <pageSetup fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.12" top="0.25" bottom="0.25" header="0.26" footer="0.25"/>
+  <pageSetup scale="98" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <oleObjects>
@@ -3356,22 +3614,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="70"/>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="71" t="s">
+      <c r="A1" s="96"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="71"/>
+      <c r="E1" s="97"/>
     </row>
     <row r="2" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="72" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
+      <c r="A2" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
     </row>
     <row r="3" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
@@ -3384,23 +3642,23 @@
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="73" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="74"/>
+      <c r="B4" s="99" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="100"/>
       <c r="D4" s="9" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
@@ -3408,8 +3666,8 @@
       <c r="A6" s="3">
         <v>2</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
@@ -3417,8 +3675,8 @@
       <c r="A7" s="3">
         <v>3</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
@@ -3426,8 +3684,8 @@
       <c r="A8" s="3">
         <v>4</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="95"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
@@ -3435,8 +3693,8 @@
       <c r="A9" s="3">
         <v>5</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="95"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
@@ -3444,8 +3702,8 @@
       <c r="A10" s="3">
         <v>6</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
+      <c r="B10" s="95"/>
+      <c r="C10" s="95"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
@@ -3453,8 +3711,8 @@
       <c r="A11" s="3">
         <v>7</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
+      <c r="B11" s="95"/>
+      <c r="C11" s="95"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
@@ -3462,8 +3720,8 @@
       <c r="A12" s="3">
         <v>8</v>
       </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="95"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
@@ -3471,8 +3729,8 @@
       <c r="A13" s="3">
         <v>9</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="95"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
@@ -3480,8 +3738,8 @@
       <c r="A14" s="3">
         <v>10</v>
       </c>
-      <c r="B14" s="69"/>
-      <c r="C14" s="69"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="95"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
@@ -3489,8 +3747,8 @@
       <c r="A15" s="3">
         <v>11</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="95"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
@@ -3498,8 +3756,8 @@
       <c r="A16" s="3">
         <v>12</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="95"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
@@ -3507,8 +3765,8 @@
       <c r="A17" s="3">
         <v>13</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="95"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
@@ -3516,8 +3774,8 @@
       <c r="A18" s="3">
         <v>14</v>
       </c>
-      <c r="B18" s="69"/>
-      <c r="C18" s="69"/>
+      <c r="B18" s="95"/>
+      <c r="C18" s="95"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
@@ -3525,8 +3783,8 @@
       <c r="A19" s="3">
         <v>15</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="69"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="95"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
@@ -3534,8 +3792,8 @@
       <c r="A20" s="3">
         <v>16</v>
       </c>
-      <c r="B20" s="69"/>
-      <c r="C20" s="69"/>
+      <c r="B20" s="95"/>
+      <c r="C20" s="95"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
@@ -3543,8 +3801,8 @@
       <c r="A21" s="3">
         <v>17</v>
       </c>
-      <c r="B21" s="69"/>
-      <c r="C21" s="69"/>
+      <c r="B21" s="95"/>
+      <c r="C21" s="95"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
@@ -3552,8 +3810,8 @@
       <c r="A22" s="3">
         <v>18</v>
       </c>
-      <c r="B22" s="69"/>
-      <c r="C22" s="69"/>
+      <c r="B22" s="95"/>
+      <c r="C22" s="95"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
@@ -3561,8 +3819,8 @@
       <c r="A23" s="3">
         <v>19</v>
       </c>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="95"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
@@ -3570,8 +3828,8 @@
       <c r="A24" s="3">
         <v>20</v>
       </c>
-      <c r="B24" s="69"/>
-      <c r="C24" s="69"/>
+      <c r="B24" s="95"/>
+      <c r="C24" s="95"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
@@ -3579,8 +3837,8 @@
       <c r="A25" s="3">
         <v>21</v>
       </c>
-      <c r="B25" s="69"/>
-      <c r="C25" s="69"/>
+      <c r="B25" s="95"/>
+      <c r="C25" s="95"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
     </row>
@@ -3588,8 +3846,8 @@
       <c r="A26" s="3">
         <v>22</v>
       </c>
-      <c r="B26" s="69"/>
-      <c r="C26" s="69"/>
+      <c r="B26" s="95"/>
+      <c r="C26" s="95"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
@@ -3597,8 +3855,8 @@
       <c r="A27" s="3">
         <v>23</v>
       </c>
-      <c r="B27" s="69"/>
-      <c r="C27" s="69"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
@@ -3606,8 +3864,8 @@
       <c r="A28" s="3">
         <v>24</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
+      <c r="B28" s="95"/>
+      <c r="C28" s="95"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
@@ -3615,8 +3873,8 @@
       <c r="A29" s="3">
         <v>25</v>
       </c>
-      <c r="B29" s="69"/>
-      <c r="C29" s="69"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="95"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
@@ -3624,8 +3882,8 @@
       <c r="A30" s="3">
         <v>26</v>
       </c>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
+      <c r="B30" s="95"/>
+      <c r="C30" s="95"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
     </row>
@@ -3633,8 +3891,8 @@
       <c r="A31" s="3">
         <v>27</v>
       </c>
-      <c r="B31" s="69"/>
-      <c r="C31" s="69"/>
+      <c r="B31" s="95"/>
+      <c r="C31" s="95"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
     </row>
@@ -3642,8 +3900,8 @@
       <c r="A32" s="3">
         <v>28</v>
       </c>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
+      <c r="B32" s="95"/>
+      <c r="C32" s="95"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
@@ -3651,8 +3909,8 @@
       <c r="A33" s="3">
         <v>29</v>
       </c>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
+      <c r="B33" s="95"/>
+      <c r="C33" s="95"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
     </row>
@@ -3660,8 +3918,8 @@
       <c r="A34" s="3">
         <v>30</v>
       </c>
-      <c r="B34" s="69"/>
-      <c r="C34" s="69"/>
+      <c r="B34" s="95"/>
+      <c r="C34" s="95"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
     </row>
@@ -3678,7 +3936,7 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>